<commit_message>
CW3MdigitalHandbook.docx - Additions to the chapter on the McKenzie Basin Wetlands Study.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_Clackamas.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_Clackamas.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4A3399-FA55-4FA4-9A50-FBEEBAA7D4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8F819E-1161-4F5B-A9A9-35EC45741E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32805" yWindow="-2865" windowWidth="23550" windowHeight="8745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="3528" windowWidth="23040" windowHeight="8748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Year</t>
   </si>
@@ -83,6 +95,9 @@
   </si>
   <si>
     <t>Baseline 2010 C97+ 11/7/20</t>
+  </si>
+  <si>
+    <t>Baseline 2010-18 C98</t>
   </si>
 </sst>
 </file>
@@ -228,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +426,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,7 +596,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -585,6 +606,8 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,23 +963,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="Q5" sqref="Q5:R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="4" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="4" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1032,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1063,7 +1086,7 @@
         <v>7.9999999999999996E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1122,7 +1145,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1178,6 +1201,65 @@
         <v>-0.54375899999999999</v>
       </c>
       <c r="S4">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>2010</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1143.6110839999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1921.3682859999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4.0370929999999996</v>
+      </c>
+      <c r="G5" s="1">
+        <v>197.01855499999999</v>
+      </c>
+      <c r="H5" s="1">
+        <v>73.459366000000003</v>
+      </c>
+      <c r="I5" s="7">
+        <v>122.410736</v>
+      </c>
+      <c r="J5" s="1">
+        <v>62.789425000000001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>717.20983899999999</v>
+      </c>
+      <c r="L5" s="1">
+        <v>75.975761000000006</v>
+      </c>
+      <c r="M5" s="7">
+        <v>999.48944100000006</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1219.0017089999999</v>
+      </c>
+      <c r="O5" s="2">
+        <v>6236.0610349999997</v>
+      </c>
+      <c r="P5" s="2">
+        <v>162867.046875</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>-387.43893400000002</v>
+      </c>
+      <c r="R5" s="8">
+        <v>-0.111915</v>
+      </c>
+      <c r="S5">
         <v>2010</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reach_Clackamas.dbf - Add attributes Q_MIN and IN_RUNOFF.
</commit_message>
<xml_diff>
--- a/DataCW3M/RegressionTesting/CW3M_Clackamas.xlsx
+++ b/DataCW3M/RegressionTesting/CW3M_Clackamas.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\RegressionTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8F819E-1161-4F5B-A9A9-35EC45741E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEC5C97-26DC-4348-9B2B-8AF8D310A6C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="3528" windowWidth="23040" windowHeight="8748" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2010" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Year</t>
   </si>
@@ -98,6 +97,12 @@
   </si>
   <si>
     <t>Baseline 2010-18 C98</t>
+  </si>
+  <si>
+    <t>Baseline 2010 C109</t>
+  </si>
+  <si>
+    <t>C109 with no springs</t>
   </si>
 </sst>
 </file>
@@ -963,23 +968,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:R5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="4" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="4" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1086,7 +1091,7 @@
         <v>7.9999999999999996E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1145,7 +1150,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1204,7 +1209,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1260,6 +1265,121 @@
         <v>-0.111915</v>
       </c>
       <c r="S5">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>2010</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1143.6110839999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1921.3682859999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.0370929999999996</v>
+      </c>
+      <c r="G6" s="1">
+        <v>197.01855499999999</v>
+      </c>
+      <c r="H6" s="1">
+        <v>73.459366000000003</v>
+      </c>
+      <c r="I6" s="7">
+        <v>105.737251</v>
+      </c>
+      <c r="J6" s="1">
+        <v>62.789425000000001</v>
+      </c>
+      <c r="K6" s="1">
+        <v>717.21026600000005</v>
+      </c>
+      <c r="L6" s="1">
+        <v>75.975761000000006</v>
+      </c>
+      <c r="M6" s="7">
+        <v>982.77160600000002</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1219.040649</v>
+      </c>
+      <c r="O6" s="2">
+        <v>6231.375</v>
+      </c>
+      <c r="P6" s="2">
+        <v>162867.046875</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>-387.443939</v>
+      </c>
+      <c r="R6" s="8">
+        <v>-0.112458</v>
+      </c>
+      <c r="S6">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>2010</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1143.6110839999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1921.3682859999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4.0370929999999996</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>73.459366000000003</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4.2416460000000002</v>
+      </c>
+      <c r="J7" s="1">
+        <v>62.789425000000001</v>
+      </c>
+      <c r="K7" s="1">
+        <v>717.21569799999997</v>
+      </c>
+      <c r="L7" s="1">
+        <v>75.975761000000006</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1078.0303960000001</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1219.301514</v>
+      </c>
+      <c r="O7" s="2">
+        <v>6231.375</v>
+      </c>
+      <c r="P7" s="2">
+        <v>162867.046875</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>6.5953189999999999</v>
+      </c>
+      <c r="R7" s="3">
+        <v>2.0960000000000002E-3</v>
+      </c>
+      <c r="S7">
         <v>2010</v>
       </c>
     </row>

</xml_diff>